<commit_message>
Update table numbers in headings
</commit_message>
<xml_diff>
--- a/reference-files/qom-template.xlsx
+++ b/reference-files/qom-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\stats\irf\18-End-of-Life\Publication\RAP Development\end-of-life-pub\reference-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliceb02\Desktop\end-of-life-pub\reference-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1529,6 +1529,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1822,6 +1823,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2115,6 +2117,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2408,6 +2411,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4467,7 +4471,7 @@
     </row>
     <row r="2" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="J2" s="82"/>
       <c r="K2" s="82"/>
@@ -32820,7 +32824,7 @@
     </row>
     <row r="2" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="J2" s="82"/>
       <c r="K2" s="82"/>
@@ -33920,7 +33924,7 @@
     </row>
     <row r="2" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="L2" s="89"/>
     </row>
@@ -34898,7 +34902,7 @@
     </row>
     <row r="2" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="L2" s="86"/>
       <c r="M2" s="89"/>

</xml_diff>